<commit_message>
Data reformatting; will work on separate branch
</commit_message>
<xml_diff>
--- a/implementation/data/borders.xlsx
+++ b/implementation/data/borders.xlsx
@@ -1,30 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sidne\OneDrive\education\cs171\CS171-Final-Project\implementation\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jovin\OneDrive\Desktop\CS171\Final Project\CS171-Final-Project\implementation\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="317" documentId="8_{F7BD6BEE-522D-4645-985D-F402F5BE1CF1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{A9E2EB43-85C2-4947-A75B-8CE47C93C552}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15F938B2-C39C-49F8-B022-1CB397751D1C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="660" yWindow="930" windowWidth="13510" windowHeight="13060" activeTab="4" xr2:uid="{AEE23E64-6203-4CD9-9423-F8877FA86498}"/>
+    <workbookView xWindow="28680" yWindow="-7455" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{AEE23E64-6203-4CD9-9423-F8877FA86498}"/>
   </bookViews>
   <sheets>
-    <sheet name="elisabeth_vallet" sheetId="5" r:id="rId1"/>
-    <sheet name="wikipedia" sheetId="6" r:id="rId2"/>
-    <sheet name="countries" sheetId="1" r:id="rId3"/>
-    <sheet name="decades" sheetId="2" r:id="rId4"/>
-    <sheet name="notes" sheetId="7" r:id="rId5"/>
+    <sheet name="aggregate_data" sheetId="8" r:id="rId1"/>
+    <sheet name="elisabeth_vallet" sheetId="5" r:id="rId2"/>
+    <sheet name="wikipedia" sheetId="6" r:id="rId3"/>
+    <sheet name="countries" sheetId="1" r:id="rId4"/>
+    <sheet name="decades" sheetId="2" r:id="rId5"/>
+    <sheet name="notes" sheetId="7" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">countries!$A$1:$E$52</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">decades!$A$1:$B$7</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">elisabeth_vallet!$A$1:$B$73</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">notes!$A$1:$E$6</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">wikipedia!$A$1:$E$41</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">countries!$A$1:$E$52</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">decades!$A$1:$B$7</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">elisabeth_vallet!$A$1:$B$73</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">notes!$A$1:$E$6</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">wikipedia!$A$1:$E$41</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -62,16 +63,10 @@
     <t>Soviet Union (East Germany)-West Germany (inner German border)</t>
   </si>
   <si>
-    <t>fascism</t>
-  </si>
-  <si>
     <t>high</t>
   </si>
   <si>
     <t>France (Algeria)-Tunisia</t>
-  </si>
-  <si>
-    <t>insurgents</t>
   </si>
   <si>
     <t>Soviet Union (East Germany)-West Germany (Berlin Wall)</t>
@@ -812,6 +807,12 @@
   </si>
   <si>
     <t>*count is taken from image of graph</t>
+  </si>
+  <si>
+    <t>Facism</t>
+  </si>
+  <si>
+    <t>Insurgents</t>
   </si>
 </sst>
 </file>
@@ -1203,22 +1204,36 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23B3C8D9-60ED-431C-BA5F-BB5B78A33916}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BD8617E-CE0E-4FD0-88B5-1396340E2F57}">
   <dimension ref="A1:B73"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0"/>
+    <sheetView topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="C70" sqref="C70"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B1" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1945</v>
       </c>
@@ -1226,7 +1241,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1946</v>
       </c>
@@ -1234,7 +1249,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>1947</v>
       </c>
@@ -1242,7 +1257,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>1948</v>
       </c>
@@ -1250,7 +1265,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>1949</v>
       </c>
@@ -1258,7 +1273,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>1950</v>
       </c>
@@ -1266,7 +1281,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>1951</v>
       </c>
@@ -1274,7 +1289,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>1952</v>
       </c>
@@ -1282,7 +1297,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>1953</v>
       </c>
@@ -1290,7 +1305,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>1954</v>
       </c>
@@ -1298,7 +1313,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>1955</v>
       </c>
@@ -1306,7 +1321,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>1956</v>
       </c>
@@ -1314,7 +1329,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>1957</v>
       </c>
@@ -1322,7 +1337,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>1958</v>
       </c>
@@ -1330,7 +1345,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>1959</v>
       </c>
@@ -1338,7 +1353,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>1960</v>
       </c>
@@ -1346,7 +1361,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>1961</v>
       </c>
@@ -1354,7 +1369,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>1962</v>
       </c>
@@ -1362,7 +1377,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>1963</v>
       </c>
@@ -1370,7 +1385,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>1964</v>
       </c>
@@ -1378,7 +1393,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>1965</v>
       </c>
@@ -1386,7 +1401,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>1966</v>
       </c>
@@ -1394,7 +1409,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>1967</v>
       </c>
@@ -1402,7 +1417,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>1968</v>
       </c>
@@ -1410,7 +1425,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>1969</v>
       </c>
@@ -1418,7 +1433,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>1970</v>
       </c>
@@ -1426,7 +1441,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>1971</v>
       </c>
@@ -1434,7 +1449,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>1972</v>
       </c>
@@ -1442,7 +1457,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>1973</v>
       </c>
@@ -1450,7 +1465,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>1974</v>
       </c>
@@ -1458,7 +1473,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>1975</v>
       </c>
@@ -1466,7 +1481,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>1976</v>
       </c>
@@ -1474,7 +1489,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>1977</v>
       </c>
@@ -1482,7 +1497,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>1978</v>
       </c>
@@ -1490,7 +1505,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>1979</v>
       </c>
@@ -1498,7 +1513,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>1980</v>
       </c>
@@ -1506,7 +1521,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>1981</v>
       </c>
@@ -1514,7 +1529,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>1982</v>
       </c>
@@ -1522,7 +1537,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>1983</v>
       </c>
@@ -1530,7 +1545,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>1984</v>
       </c>
@@ -1538,7 +1553,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>1985</v>
       </c>
@@ -1546,7 +1561,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>1986</v>
       </c>
@@ -1554,7 +1569,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>1987</v>
       </c>
@@ -1562,7 +1577,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>1988</v>
       </c>
@@ -1570,7 +1585,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>1989</v>
       </c>
@@ -1578,7 +1593,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>1990</v>
       </c>
@@ -1586,7 +1601,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>1991</v>
       </c>
@@ -1594,7 +1609,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>1992</v>
       </c>
@@ -1602,7 +1617,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>1993</v>
       </c>
@@ -1610,7 +1625,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>1994</v>
       </c>
@@ -1618,7 +1633,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>1995</v>
       </c>
@@ -1626,7 +1641,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>1996</v>
       </c>
@@ -1634,7 +1649,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>1997</v>
       </c>
@@ -1642,7 +1657,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>1998</v>
       </c>
@@ -1650,7 +1665,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>1999</v>
       </c>
@@ -1658,7 +1673,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>2000</v>
       </c>
@@ -1666,7 +1681,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>2001</v>
       </c>
@@ -1674,7 +1689,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>2002</v>
       </c>
@@ -1682,7 +1697,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>2003</v>
       </c>
@@ -1690,7 +1705,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>2004</v>
       </c>
@@ -1698,7 +1713,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>2005</v>
       </c>
@@ -1706,7 +1721,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>2006</v>
       </c>
@@ -1714,7 +1729,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>2007</v>
       </c>
@@ -1722,7 +1737,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>2008</v>
       </c>
@@ -1730,7 +1745,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>2009</v>
       </c>
@@ -1738,7 +1753,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>2010</v>
       </c>
@@ -1746,7 +1761,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>2011</v>
       </c>
@@ -1754,7 +1769,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>2012</v>
       </c>
@@ -1762,7 +1777,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>2013</v>
       </c>
@@ -1770,7 +1785,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>2014</v>
       </c>
@@ -1778,7 +1793,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>2015</v>
       </c>
@@ -1786,7 +1801,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>2016</v>
       </c>
@@ -1800,42 +1815,42 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4AE1B37-B90D-4B6D-86F5-429437F69441}">
   <dimension ref="A1:E41"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A19" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="31.26953125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="34.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.81640625" customWidth="1"/>
+    <col min="1" max="1" width="31.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C1" t="s">
         <v>103</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>104</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>105</v>
       </c>
-      <c r="D1" t="s">
-        <v>106</v>
-      </c>
-      <c r="E1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B2" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="C2">
         <v>1953</v>
@@ -1844,15 +1859,15 @@
         <v>248</v>
       </c>
       <c r="E2" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B3" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="C3">
         <v>1975</v>
@@ -1861,15 +1876,15 @@
         <v>120</v>
       </c>
       <c r="E3" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B4" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C4">
         <v>1991</v>
@@ -1878,32 +1893,32 @@
         <v>193</v>
       </c>
       <c r="E4" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B5" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C5">
         <v>1994</v>
       </c>
       <c r="D5" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E5" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B6" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C6">
         <v>1998</v>
@@ -1912,15 +1927,15 @@
         <v>11</v>
       </c>
       <c r="E6" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B7" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C7">
         <v>1999</v>
@@ -1929,15 +1944,15 @@
         <v>870</v>
       </c>
       <c r="E7" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B8" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C8">
         <v>2001</v>
@@ -1946,15 +1961,15 @@
         <v>8</v>
       </c>
       <c r="E8" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B9" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="C9">
         <v>2001</v>
@@ -1963,15 +1978,15 @@
         <v>1700</v>
       </c>
       <c r="E9" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B10" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="C10">
         <v>2001</v>
@@ -1980,15 +1995,15 @@
         <v>209</v>
       </c>
       <c r="E10" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B11" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C11">
         <v>2003</v>
@@ -1997,15 +2012,15 @@
         <v>500</v>
       </c>
       <c r="E11" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B12" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C12">
         <v>2004</v>
@@ -2014,15 +2029,15 @@
         <v>550</v>
       </c>
       <c r="E12" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B13" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="C13">
         <v>2004</v>
@@ -2031,15 +2046,15 @@
         <v>75</v>
       </c>
       <c r="E13" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B14" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C14">
         <v>2005</v>
@@ -2048,15 +2063,15 @@
         <v>20</v>
       </c>
       <c r="E14" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B15" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C15">
         <v>2006</v>
@@ -2065,15 +2080,15 @@
         <v>45</v>
       </c>
       <c r="E15" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B16" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C16">
         <v>2013</v>
@@ -2082,15 +2097,15 @@
         <v>245</v>
       </c>
       <c r="E16" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
-        <v>116</v>
-      </c>
       <c r="B17" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C17">
         <v>2014</v>
@@ -2099,15 +2114,15 @@
         <v>30</v>
       </c>
       <c r="E17" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B18" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="C18">
         <v>2014</v>
@@ -2116,15 +2131,15 @@
         <v>900</v>
       </c>
       <c r="E18" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B19" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C19">
         <v>2015</v>
@@ -2133,15 +2148,15 @@
         <v>30</v>
       </c>
       <c r="E19" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B20" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C20">
         <v>2015</v>
@@ -2150,15 +2165,15 @@
         <v>175</v>
       </c>
       <c r="E20" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B21" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C21">
         <v>2015</v>
@@ -2167,15 +2182,15 @@
         <v>41</v>
       </c>
       <c r="E21" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B22" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="C22">
         <v>2018</v>
@@ -2184,330 +2199,330 @@
         <v>11</v>
       </c>
       <c r="E22" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
+        <v>118</v>
+      </c>
+      <c r="B23" t="s">
+        <v>119</v>
+      </c>
+      <c r="C23" t="s">
         <v>120</v>
-      </c>
-      <c r="B23" t="s">
-        <v>121</v>
-      </c>
-      <c r="C23" t="s">
-        <v>122</v>
       </c>
       <c r="D23">
         <v>32</v>
       </c>
       <c r="E23" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
+        <v>126</v>
+      </c>
+      <c r="B24" t="s">
+        <v>127</v>
+      </c>
+      <c r="C24" t="s">
         <v>128</v>
-      </c>
-      <c r="B24" t="s">
-        <v>129</v>
-      </c>
-      <c r="C24" t="s">
-        <v>130</v>
       </c>
       <c r="D24">
         <v>3.1</v>
       </c>
       <c r="E24" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
+        <v>154</v>
+      </c>
+      <c r="B25" t="s">
+        <v>155</v>
+      </c>
+      <c r="C25" t="s">
         <v>156</v>
-      </c>
-      <c r="B25" t="s">
-        <v>157</v>
-      </c>
-      <c r="C25" t="s">
-        <v>158</v>
       </c>
       <c r="D25">
         <v>225</v>
       </c>
       <c r="E25" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
+        <v>182</v>
+      </c>
+      <c r="B26" t="s">
+        <v>183</v>
+      </c>
+      <c r="C26" t="s">
         <v>184</v>
-      </c>
-      <c r="B26" t="s">
-        <v>185</v>
-      </c>
-      <c r="C26" t="s">
-        <v>186</v>
       </c>
       <c r="D26">
         <v>708</v>
       </c>
       <c r="E26" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
+        <v>176</v>
+      </c>
+      <c r="B27" t="s">
+        <v>177</v>
+      </c>
+      <c r="C27" t="s">
         <v>178</v>
-      </c>
-      <c r="B27" t="s">
-        <v>179</v>
-      </c>
-      <c r="C27" t="s">
-        <v>180</v>
       </c>
       <c r="D27">
         <v>100</v>
       </c>
       <c r="E27" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
+        <v>130</v>
+      </c>
+      <c r="B28" t="s">
+        <v>194</v>
+      </c>
+      <c r="C28" t="s">
+        <v>131</v>
+      </c>
+      <c r="D28" t="s">
         <v>132</v>
       </c>
-      <c r="B28" t="s">
-        <v>196</v>
-      </c>
-      <c r="C28" t="s">
+      <c r="E28" t="s">
         <v>133</v>
       </c>
-      <c r="D28" t="s">
-        <v>134</v>
-      </c>
-      <c r="E28" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
+        <v>121</v>
+      </c>
+      <c r="B29" t="s">
+        <v>122</v>
+      </c>
+      <c r="C29" t="s">
         <v>123</v>
       </c>
-      <c r="B29" t="s">
-        <v>124</v>
-      </c>
-      <c r="C29" t="s">
-        <v>125</v>
-      </c>
       <c r="D29" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E29" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B30" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C30" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D30">
         <v>650</v>
       </c>
       <c r="E30" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
+        <v>106</v>
+      </c>
+      <c r="B31" t="s">
+        <v>107</v>
+      </c>
+      <c r="C31" t="s">
         <v>108</v>
       </c>
-      <c r="B31" t="s">
+      <c r="D31" t="s">
         <v>109</v>
       </c>
-      <c r="C31" t="s">
+      <c r="E31" t="s">
         <v>110</v>
       </c>
-      <c r="D31" t="s">
-        <v>111</v>
-      </c>
-      <c r="E31" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B32" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C32" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="D32" s="1">
         <v>1416</v>
       </c>
       <c r="E32" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B33" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C33" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="D33" s="1">
         <v>3268</v>
       </c>
       <c r="E33" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B34" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C34" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="D34" s="1">
         <v>1624</v>
       </c>
       <c r="E34" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B35" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C35" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="D35">
         <v>700</v>
       </c>
       <c r="E35" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B36" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C36" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="D36" s="1">
         <v>2400</v>
       </c>
       <c r="E36" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
+        <v>165</v>
+      </c>
+      <c r="B37" t="s">
+        <v>166</v>
+      </c>
+      <c r="C37" t="s">
         <v>167</v>
-      </c>
-      <c r="B37" t="s">
-        <v>168</v>
-      </c>
-      <c r="C37" t="s">
-        <v>169</v>
       </c>
       <c r="D37">
         <v>179</v>
       </c>
       <c r="E37" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B38" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C38" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="D38">
         <v>828</v>
       </c>
       <c r="E38" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B39" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C39" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="D39">
         <v>144</v>
       </c>
       <c r="E39" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B40" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="C40" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="D40" s="1">
         <v>2000</v>
       </c>
       <c r="E40" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B41" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C41" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="D41">
         <v>410</v>
       </c>
       <c r="E41" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
   </sheetData>
@@ -2520,22 +2535,24 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68D509FD-693C-48E9-8A47-16C134ACAA4F}">
   <dimension ref="A1:E52"/>
   <sheetViews>
-    <sheetView topLeftCell="A43" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="B36" sqref="B36"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="58.08984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.36328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.26953125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="29.26953125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="58.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29.21875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2552,7 +2569,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -2563,15 +2580,15 @@
         <v>845</v>
       </c>
       <c r="D2" t="s">
+        <v>229</v>
+      </c>
+      <c r="E2" t="s">
         <v>6</v>
       </c>
-      <c r="E2" t="s">
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>8</v>
       </c>
       <c r="B3">
         <v>1957</v>
@@ -2580,15 +2597,15 @@
         <v>171</v>
       </c>
       <c r="D3" t="s">
-        <v>9</v>
+        <v>230</v>
       </c>
       <c r="E3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B4">
         <v>1961</v>
@@ -2597,101 +2614,101 @@
         <v>93</v>
       </c>
       <c r="D4" t="s">
+        <v>229</v>
+      </c>
+      <c r="E4" t="s">
         <v>6</v>
       </c>
-      <c r="E4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" t="s">
         <v>11</v>
       </c>
-      <c r="B5" t="s">
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
         <v>12</v>
-      </c>
-      <c r="E5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>14</v>
       </c>
       <c r="B6">
         <v>1976</v>
       </c>
       <c r="E6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
+      <c r="E7" t="s">
         <v>16</v>
       </c>
-      <c r="B7" t="s">
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
         <v>17</v>
       </c>
-      <c r="E7" t="s">
+      <c r="B8" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
+      <c r="E8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
         <v>19</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B9" t="s">
         <v>20</v>
-      </c>
-      <c r="E8" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>21</v>
-      </c>
-      <c r="B9" t="s">
-        <v>22</v>
       </c>
       <c r="C9">
         <v>114</v>
       </c>
       <c r="E9" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B10">
         <v>1980</v>
       </c>
       <c r="C10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" t="s">
+        <v>23</v>
+      </c>
+      <c r="E10" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
         <v>24</v>
       </c>
-      <c r="D10" t="s">
+      <c r="B11" t="s">
         <v>25</v>
       </c>
-      <c r="E10" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
+      <c r="E11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
         <v>26</v>
-      </c>
-      <c r="B11" t="s">
-        <v>27</v>
-      </c>
-      <c r="E11" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
-        <v>28</v>
       </c>
       <c r="B12">
         <v>1982</v>
@@ -2700,140 +2717,140 @@
         <v>7</v>
       </c>
       <c r="D12" t="s">
+        <v>27</v>
+      </c>
+      <c r="E12" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>28</v>
+      </c>
+      <c r="B13" t="s">
         <v>29</v>
       </c>
-      <c r="E12" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
+      <c r="E13" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
         <v>30</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B14" t="s">
         <v>31</v>
       </c>
-      <c r="E13" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
+      <c r="E14" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
         <v>32</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B15" t="s">
         <v>33</v>
-      </c>
-      <c r="E14" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
-        <v>34</v>
-      </c>
-      <c r="B15" t="s">
-        <v>35</v>
       </c>
       <c r="C15">
         <v>301</v>
       </c>
       <c r="D15" t="s">
+        <v>34</v>
+      </c>
+      <c r="E15" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
         <v>36</v>
       </c>
-      <c r="E15" t="s">
+      <c r="B16" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
+      <c r="E16" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
         <v>38</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B17" t="s">
         <v>39</v>
       </c>
-      <c r="E16" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
+      <c r="E17" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
         <v>40</v>
-      </c>
-      <c r="B17" t="s">
-        <v>41</v>
-      </c>
-      <c r="E17" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
-        <v>42</v>
       </c>
       <c r="B18">
         <v>1989</v>
       </c>
       <c r="E18" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B19">
         <v>1989</v>
       </c>
       <c r="E19" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A20" t="s">
+      <c r="B20" t="s">
+        <v>44</v>
+      </c>
+      <c r="D20" t="s">
         <v>45</v>
       </c>
-      <c r="B20" t="s">
+      <c r="E20" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
         <v>46</v>
       </c>
-      <c r="D20" t="s">
+      <c r="B21" t="s">
         <v>47</v>
       </c>
-      <c r="E20" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A21" t="s">
+      <c r="D21" t="s">
+        <v>27</v>
+      </c>
+      <c r="E21" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
         <v>48</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B22" t="s">
         <v>49</v>
       </c>
-      <c r="D21" t="s">
-        <v>29</v>
-      </c>
-      <c r="E21" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A22" t="s">
+      <c r="D22" t="s">
         <v>50</v>
       </c>
-      <c r="B22" t="s">
+      <c r="E22" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
         <v>51</v>
-      </c>
-      <c r="D22" t="s">
-        <v>52</v>
-      </c>
-      <c r="E22" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A23" t="s">
-        <v>53</v>
       </c>
       <c r="B23">
         <v>1994</v>
@@ -2842,15 +2859,15 @@
         <v>31</v>
       </c>
       <c r="D23" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E23" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B24">
         <v>1994</v>
@@ -2859,12 +2876,12 @@
         <v>122</v>
       </c>
       <c r="E24" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B25">
         <v>1995</v>
@@ -2873,12 +2890,12 @@
         <v>5</v>
       </c>
       <c r="E25" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B26">
         <v>1998</v>
@@ -2887,96 +2904,96 @@
         <v>6</v>
       </c>
       <c r="E26" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B27">
         <v>1999</v>
       </c>
       <c r="E27" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
+        <v>57</v>
+      </c>
+      <c r="B28" t="s">
+        <v>58</v>
+      </c>
+      <c r="D28" t="s">
         <v>59</v>
       </c>
-      <c r="B28" t="s">
+      <c r="E28" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
         <v>60</v>
       </c>
-      <c r="D28" t="s">
+      <c r="B29" t="s">
+        <v>58</v>
+      </c>
+      <c r="C29" t="s">
         <v>61</v>
       </c>
-      <c r="E28" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A29" t="s">
+      <c r="E29" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
         <v>62</v>
       </c>
-      <c r="B29" t="s">
-        <v>60</v>
-      </c>
-      <c r="C29" t="s">
+      <c r="B30" t="s">
+        <v>58</v>
+      </c>
+      <c r="C30" t="s">
         <v>63</v>
       </c>
-      <c r="E29" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A30" t="s">
+      <c r="E30" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
         <v>64</v>
-      </c>
-      <c r="B30" t="s">
-        <v>60</v>
-      </c>
-      <c r="C30" t="s">
-        <v>65</v>
-      </c>
-      <c r="E30" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A31" t="s">
-        <v>66</v>
       </c>
       <c r="B31">
         <v>2001</v>
       </c>
       <c r="C31" t="s">
+        <v>65</v>
+      </c>
+      <c r="D31" t="s">
+        <v>66</v>
+      </c>
+      <c r="E31" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
         <v>67</v>
       </c>
-      <c r="D31" t="s">
+      <c r="B32" t="s">
         <v>68</v>
-      </c>
-      <c r="E31" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A32" t="s">
-        <v>69</v>
-      </c>
-      <c r="B32" t="s">
-        <v>70</v>
       </c>
       <c r="C32">
         <v>82</v>
       </c>
       <c r="E32" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B33">
         <v>2002</v>
@@ -2985,15 +3002,15 @@
         <v>245</v>
       </c>
       <c r="D33" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E33" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B34">
         <v>2003</v>
@@ -3002,82 +3019,82 @@
         <v>300</v>
       </c>
       <c r="D34" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E34" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B35">
         <v>2003</v>
       </c>
       <c r="C35" t="s">
+        <v>73</v>
+      </c>
+      <c r="D35" t="s">
+        <v>74</v>
+      </c>
+      <c r="E35" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
         <v>75</v>
       </c>
-      <c r="D35" t="s">
+      <c r="B36" t="s">
         <v>76</v>
       </c>
-      <c r="E35" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A36" t="s">
+      <c r="E36" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
         <v>77</v>
-      </c>
-      <c r="B36" t="s">
-        <v>78</v>
-      </c>
-      <c r="E36" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A37" t="s">
-        <v>79</v>
       </c>
       <c r="B37">
         <v>2004</v>
       </c>
       <c r="E37" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B38">
         <v>2006</v>
       </c>
       <c r="E38" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B39">
         <v>2006</v>
       </c>
       <c r="C39" t="s">
+        <v>80</v>
+      </c>
+      <c r="D39" t="s">
+        <v>81</v>
+      </c>
+      <c r="E39" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
         <v>82</v>
-      </c>
-      <c r="D39" t="s">
-        <v>83</v>
-      </c>
-      <c r="E39" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A40" t="s">
-        <v>84</v>
       </c>
       <c r="B40">
         <v>2007</v>
@@ -3086,60 +3103,60 @@
         <v>613</v>
       </c>
       <c r="D40" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E40" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B41">
         <v>2007</v>
       </c>
       <c r="C41" t="s">
+        <v>85</v>
+      </c>
+      <c r="D41" t="s">
+        <v>86</v>
+      </c>
+      <c r="E41" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
         <v>87</v>
-      </c>
-      <c r="D41" t="s">
-        <v>88</v>
-      </c>
-      <c r="E41" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A42" t="s">
-        <v>89</v>
       </c>
       <c r="B42">
         <v>2008</v>
       </c>
       <c r="C42" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D42" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E42" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B43">
         <v>2009</v>
       </c>
       <c r="E43" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B44">
         <v>2009</v>
@@ -3148,54 +3165,54 @@
         <v>7</v>
       </c>
       <c r="E44" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B45">
         <v>2010</v>
       </c>
       <c r="D45" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E45" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B46">
         <v>2010</v>
       </c>
       <c r="D46" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E46" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B47">
         <v>2010</v>
       </c>
       <c r="D47" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E47" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B48">
         <v>2012</v>
@@ -3204,12 +3221,12 @@
         <v>1</v>
       </c>
       <c r="E48" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B49">
         <v>2012</v>
@@ -3218,40 +3235,40 @@
         <v>8</v>
       </c>
       <c r="E49" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B50">
         <v>2012</v>
       </c>
       <c r="E50" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B51">
         <v>2013</v>
       </c>
       <c r="E51" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B52">
         <v>2014</v>
       </c>
       <c r="E52" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -3261,25 +3278,25 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F6909C5-C69F-4C62-8A7B-EBE2836EADA3}">
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="A1:B7"/>
+      <selection activeCell="B2" sqref="B2:B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B1" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1950</v>
       </c>
@@ -3287,7 +3304,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1960</v>
       </c>
@@ -3295,7 +3312,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>1970</v>
       </c>
@@ -3303,7 +3320,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>1980</v>
       </c>
@@ -3311,7 +3328,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>1990</v>
       </c>
@@ -3319,7 +3336,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>2000</v>
       </c>
@@ -3333,102 +3350,103 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D7E4327-AADE-41D1-9C71-2A07C3F8760F}">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.90625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="47.7265625" customWidth="1"/>
+    <col min="1" max="1" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="47.77734375" customWidth="1"/>
+    <col min="3" max="3" width="20.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>210</v>
+      </c>
+      <c r="B1" t="s">
+        <v>208</v>
+      </c>
+      <c r="C1" t="s">
+        <v>209</v>
+      </c>
+      <c r="D1" t="s">
+        <v>226</v>
+      </c>
+      <c r="E1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>211</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>212</v>
       </c>
-      <c r="B1" t="s">
-        <v>210</v>
-      </c>
-      <c r="C1" t="s">
-        <v>211</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="D2" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="E2" t="s">
         <v>228</v>
       </c>
-      <c r="E1" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>213</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>221</v>
-      </c>
-      <c r="C2" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>214</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="C3" s="3" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>216</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>223</v>
       </c>
-      <c r="E2" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>215</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>216</v>
-      </c>
-      <c r="C3" s="3" t="s">
+      <c r="E4" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>217</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
+      <c r="B5" s="2" t="s">
         <v>218</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="C5" s="3" t="s">
+        <v>223</v>
+      </c>
+      <c r="E5" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>222</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>220</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C6" s="3" t="s">
         <v>225</v>
-      </c>
-      <c r="E4" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>219</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>220</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>225</v>
-      </c>
-      <c r="E5" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>224</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>222</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>227</v>
       </c>
     </row>
   </sheetData>

</xml_diff>